<commit_message>
Commit for runing Build through Jenkins
</commit_message>
<xml_diff>
--- a/Resource/TestCasesFile.xlsx
+++ b/Resource/TestCasesFile.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EXITS TEST\Flipkart\Flipkart\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EXITS TEST\Flipkart\Flipkart\Resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4403672E-1563-4247-B480-F87B66183019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88337D1F-48A5-4B60-8F68-EC0EDF556BAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="64">
   <si>
     <t>name</t>
   </si>
@@ -213,15 +213,9 @@
     <t>addtoCartOutofStock</t>
   </si>
   <si>
-    <t>deletefromCart</t>
-  </si>
-  <si>
     <t>addToCart</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>iphone 13 se 128</t>
   </si>
   <si>
@@ -229,6 +223,9 @@
   </si>
   <si>
     <t>dropDownElectronics</t>
+  </si>
+  <si>
+    <t>verifyTitle</t>
   </si>
 </sst>
 </file>
@@ -878,10 +875,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F0F6099-DB78-4330-8844-85826A4C96A8}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="A1:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -907,12 +904,12 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
         <v>48</v>
@@ -929,7 +926,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
         <v>48</v>
@@ -940,22 +937,8 @@
       <c r="D3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" t="s">
-        <v>62</v>
+      <c r="E3" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1035,10 +1018,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEC1FDB6-6D98-4AAD-84B9-4D68F883C6B7}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1055,25 +1038,23 @@
       <c r="B1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
         <v>48</v>
       </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1261,7 +1242,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3697BF9-5781-42B5-9705-AC1492885E8B}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>

</xml_diff>